<commit_message>
Changed CoA implementation to handle multiple file creations at the same time!
</commit_message>
<xml_diff>
--- a/automation/src/res/Western-Biologics Part Number to ProdCode.xlsx
+++ b/automation/src/res/Western-Biologics Part Number to ProdCode.xlsx
@@ -947,13 +947,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -994,6 +994,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1008,25 +1011,19 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1034,6 +1031,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1345,10 +1345,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="91.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="91.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="12.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1361,2479 +1361,2479 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="D2" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="D3" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="D4" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="D5" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="D6" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="D7" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="D8" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="D9" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="D10" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="D11" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="D12" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="D13" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="D14" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="D15" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="D16" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="D17" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="D18" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="D19" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="D20" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="D21" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="D22" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="D23" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="A29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="A33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="A38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="4" t="s">
+      <c r="A39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="4" t="s">
+      <c r="A41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" s="7" t="s">
+      <c r="A42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B43" s="7" t="s">
+      <c r="A43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="7" t="s">
+      <c r="A44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" s="7" t="s">
+      <c r="A45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="7" t="s">
+      <c r="A46" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" s="7" t="s">
+      <c r="A47" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="7" t="s">
+      <c r="A48" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="7" t="s">
+      <c r="A49" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="7" t="s">
+      <c r="A50" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="D50" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="7" t="s">
+      <c r="A51" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>64</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="3"/>
+      <c r="D51" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" s="7" t="s">
+      <c r="A52" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>65</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D52" s="3"/>
+      <c r="D52" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="7" t="s">
+      <c r="A53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="3"/>
+      <c r="D53" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B54" s="7" t="s">
+      <c r="A54" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="3"/>
+      <c r="D54" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" s="7" t="s">
+      <c r="A55" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D55" s="3"/>
+      <c r="D55" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B56" s="7" t="s">
+      <c r="A56" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D56" s="3"/>
+      <c r="D56" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57" s="7" t="s">
+      <c r="A57" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>70</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58" s="7" t="s">
+      <c r="A58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D58" s="3"/>
+      <c r="D58" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B59" s="7" t="s">
+      <c r="A59" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="3"/>
+      <c r="D59" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="7" t="s">
+      <c r="A60" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D60" s="3"/>
+      <c r="D60" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B61" s="7" t="s">
+      <c r="A61" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>75</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D61" s="3"/>
+      <c r="D61" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" s="7" t="s">
+      <c r="A62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>77</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="3"/>
+      <c r="D62" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B63" s="7" t="s">
+      <c r="A63" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D63" s="3"/>
+      <c r="D63" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B64" s="7" t="s">
+      <c r="A64" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D64" s="3"/>
+      <c r="D64" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B65" s="7" t="s">
+      <c r="A65" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>83</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D65" s="3"/>
+      <c r="D65" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B66" s="7" t="s">
+      <c r="A66" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D66" s="3"/>
+      <c r="D66" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
-      <c r="A67" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B67" s="7" t="s">
+      <c r="A67" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>85</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D67" s="3"/>
+      <c r="D67" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
-      <c r="A68" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" s="7" t="s">
+      <c r="A68" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D68" s="3"/>
+      <c r="D68" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B69" s="7" t="s">
+      <c r="A69" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D69" s="3"/>
+      <c r="D69" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
-      <c r="A70" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B70" s="7" t="s">
+      <c r="A70" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B70" s="8" t="s">
         <v>88</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D70" s="3"/>
+      <c r="D70" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
-      <c r="A71" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71" s="7" t="s">
+      <c r="A71" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>89</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D71" s="3"/>
+      <c r="D71" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
-      <c r="A72" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72" s="7" t="s">
+      <c r="A72" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D72" s="3"/>
+      <c r="D72" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
-      <c r="A73" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B73" s="7" t="s">
+      <c r="A73" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D73" s="3"/>
+      <c r="D73" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
-      <c r="A74" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74" s="7" t="s">
+      <c r="A74" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D74" s="3"/>
+      <c r="D74" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
-      <c r="A75" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B75" s="7" t="s">
+      <c r="A75" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>95</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D75" s="3"/>
+      <c r="D75" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
-      <c r="A76" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B76" s="7" t="s">
+      <c r="A76" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>97</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D76" s="3"/>
+      <c r="D76" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B77" s="7" t="s">
+      <c r="A77" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>98</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D77" s="3"/>
+      <c r="D77" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
-      <c r="A78" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B78" s="7" t="s">
+      <c r="A78" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" s="8" t="s">
         <v>99</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D78" s="3"/>
+      <c r="D78" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B79" s="7" t="s">
+      <c r="A79" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D79" s="3"/>
+      <c r="D79" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
-      <c r="A80" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B80" s="7" t="s">
+      <c r="A80" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>102</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D80" s="3"/>
+      <c r="D80" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
-      <c r="A81" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B81" s="7" t="s">
+      <c r="A81" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>103</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D81" s="3"/>
+      <c r="D81" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
-      <c r="A82" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B82" s="7" t="s">
+      <c r="A82" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D82" s="3"/>
+      <c r="D82" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
-      <c r="A83" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B83" s="7" t="s">
+      <c r="A83" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>106</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D83" s="3"/>
+      <c r="D83" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
-      <c r="A84" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B84" s="7" t="s">
+      <c r="A84" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>108</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D84" s="3"/>
+      <c r="D84" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
-      <c r="A85" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B85" s="7" t="s">
+      <c r="A85" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>110</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D85" s="3"/>
+      <c r="D85" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
-      <c r="A86" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B86" s="7" t="s">
+      <c r="A86" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>111</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D86" s="3"/>
+      <c r="D86" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
-      <c r="A87" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B87" s="7" t="s">
+      <c r="A87" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B87" s="8" t="s">
         <v>112</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D87" s="3"/>
+      <c r="D87" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
-      <c r="A88" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B88" s="7" t="s">
+      <c r="A88" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B88" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D88" s="3"/>
+      <c r="D88" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
-      <c r="A89" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B89" s="7" t="s">
+      <c r="A89" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="8" t="s">
         <v>114</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D89" s="3"/>
+      <c r="D89" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
-      <c r="A90" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B90" s="7" t="s">
+      <c r="A90" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B90" s="8" t="s">
         <v>115</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
-      <c r="A91" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B91" s="7" t="s">
+      <c r="A91" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B91" s="8" t="s">
         <v>116</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
-      <c r="A92" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B92" s="7" t="s">
+      <c r="A92" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>117</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
-      <c r="A93" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B93" s="7" t="s">
+      <c r="A93" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B93" s="8" t="s">
         <v>118</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D93" s="3"/>
+      <c r="D93" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
-      <c r="A94" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B94" s="7" t="s">
+      <c r="A94" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>120</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D94" s="3"/>
+      <c r="D94" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
-      <c r="A95" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B95" s="7" t="s">
+      <c r="A95" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B95" s="8" t="s">
         <v>122</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D95" s="3"/>
+      <c r="D95" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
-      <c r="A96" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B96" s="7" t="s">
+      <c r="A96" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>124</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D96" s="3"/>
+      <c r="D96" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B97" s="7" t="s">
+      <c r="A97" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>124</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D97" s="3"/>
+      <c r="D97" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
-      <c r="A98" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B98" s="7" t="s">
+      <c r="A98" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B98" s="8" t="s">
         <v>126</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D98" s="3"/>
+      <c r="D98" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
-      <c r="A99" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B99" s="7" t="s">
+      <c r="A99" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B99" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D99" s="3"/>
+      <c r="D99" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
-      <c r="A100" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B100" s="7" t="s">
+      <c r="A100" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B100" s="8" t="s">
         <v>129</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D100" s="3"/>
+      <c r="D100" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
-      <c r="A101" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B101" s="7" t="s">
+      <c r="A101" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>130</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D101" s="3"/>
+      <c r="D101" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
-      <c r="A102" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B102" s="7" t="s">
+      <c r="A102" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>132</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D102" s="3"/>
+      <c r="D102" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
-      <c r="A103" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B103" s="7" t="s">
+      <c r="A103" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D103" s="3"/>
+      <c r="D103" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
-      <c r="A104" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B104" s="7" t="s">
+      <c r="A104" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>135</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D104" s="3"/>
+      <c r="D104" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
-      <c r="A105" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B105" s="7" t="s">
+      <c r="A105" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>137</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D105" s="3"/>
+      <c r="D105" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
-      <c r="A106" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B106" s="7" t="s">
+      <c r="A106" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>139</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D106" s="3"/>
+      <c r="D106" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
-      <c r="A107" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B107" s="7" t="s">
+      <c r="A107" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>141</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D107" s="3"/>
+      <c r="D107" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
-      <c r="A108" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B108" s="7" t="s">
+      <c r="A108" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>143</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D108" s="3"/>
+      <c r="D108" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
-      <c r="A109" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B109" s="7" t="s">
+      <c r="A109" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>144</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D109" s="3"/>
+      <c r="D109" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
-      <c r="A110" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B110" s="7" t="s">
+      <c r="A110" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>145</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D110" s="3"/>
+      <c r="D110" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
-      <c r="A111" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B111" s="7" t="s">
+      <c r="A111" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>147</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D111" s="3"/>
+      <c r="D111" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
-      <c r="A112" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B112" s="7" t="s">
+      <c r="A112" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>149</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D112" s="3"/>
+      <c r="D112" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
-      <c r="A113" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B113" s="7" t="s">
+      <c r="A113" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B113" s="8" t="s">
         <v>151</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D113" s="3"/>
+      <c r="D113" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
-      <c r="A114" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B114" s="7" t="s">
+      <c r="A114" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>152</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D114" s="3"/>
+      <c r="D114" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
-      <c r="A115" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B115" s="7" t="s">
+      <c r="A115" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B115" s="8" t="s">
         <v>153</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D115" s="3"/>
+      <c r="D115" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
-      <c r="A116" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B116" s="7" t="s">
+      <c r="A116" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>155</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D116" s="3"/>
+      <c r="D116" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
-      <c r="A117" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B117" s="7" t="s">
+      <c r="A117" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>157</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D117" s="3"/>
+      <c r="D117" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
-      <c r="A118" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B118" s="7" t="s">
+      <c r="A118" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>158</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D118" s="3"/>
+      <c r="D118" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
-      <c r="A119" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B119" s="7" t="s">
+      <c r="A119" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>160</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D119" s="3"/>
+      <c r="D119" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
-      <c r="A120" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B120" s="7" t="s">
+      <c r="A120" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>162</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D120" s="3"/>
+      <c r="D120" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
-      <c r="A121" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B121" s="7" t="s">
+      <c r="A121" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B121" s="8" t="s">
         <v>164</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D121" s="3"/>
+      <c r="D121" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
-      <c r="A122" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B122" s="7" t="s">
+      <c r="A122" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B122" s="8" t="s">
         <v>166</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D122" s="3"/>
+      <c r="D122" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
-      <c r="A123" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B123" s="7" t="s">
+      <c r="A123" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B123" s="8" t="s">
         <v>168</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D123" s="3"/>
+      <c r="D123" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
-      <c r="A124" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B124" s="7" t="s">
+      <c r="A124" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B124" s="8" t="s">
         <v>170</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D124" s="3"/>
+      <c r="D124" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
-      <c r="A125" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B125" s="7" t="s">
+      <c r="A125" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B125" s="8" t="s">
         <v>171</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D125" s="3"/>
+      <c r="D125" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
-      <c r="A126" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B126" s="7" t="s">
+      <c r="A126" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B126" s="8" t="s">
         <v>173</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D126" s="3"/>
+      <c r="D126" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
-      <c r="A127" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B127" s="7" t="s">
+      <c r="A127" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B127" s="8" t="s">
         <v>175</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D127" s="3"/>
+      <c r="D127" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
-      <c r="A128" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B128" s="7" t="s">
+      <c r="A128" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>177</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D128" s="3"/>
+      <c r="D128" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
-      <c r="A129" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B129" s="7" t="s">
+      <c r="A129" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B129" s="8" t="s">
         <v>179</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D129" s="3"/>
+      <c r="D129" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
-      <c r="A130" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B130" s="7" t="s">
+      <c r="A130" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>181</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D130" s="3"/>
+      <c r="D130" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
-      <c r="A131" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B131" s="7" t="s">
+      <c r="A131" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B131" s="8" t="s">
         <v>183</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D131" s="3"/>
+      <c r="D131" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
-      <c r="A132" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B132" s="7" t="s">
+      <c r="A132" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B132" s="8" t="s">
         <v>185</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D132" s="3"/>
+      <c r="D132" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
-      <c r="A133" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B133" s="7" t="s">
+      <c r="A133" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B133" s="8" t="s">
         <v>187</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D133" s="3"/>
+      <c r="D133" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
-      <c r="A134" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B134" s="7" t="s">
+      <c r="A134" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B134" s="8" t="s">
         <v>188</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D134" s="3"/>
+      <c r="D134" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
-      <c r="A135" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B135" s="7" t="s">
+      <c r="A135" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B135" s="8" t="s">
         <v>190</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D135" s="3"/>
+      <c r="D135" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
-      <c r="A136" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B136" s="7" t="s">
+      <c r="A136" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B136" s="8" t="s">
         <v>192</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D136" s="3"/>
+      <c r="D136" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
-      <c r="A137" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B137" s="7" t="s">
+      <c r="A137" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B137" s="8" t="s">
         <v>194</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D137" s="3"/>
+      <c r="D137" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
-      <c r="A138" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B138" s="7" t="s">
+      <c r="A138" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B138" s="8" t="s">
         <v>196</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D138" s="3"/>
+      <c r="D138" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
-      <c r="A139" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B139" s="7" t="s">
+      <c r="A139" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B139" s="8" t="s">
         <v>198</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D139" s="3"/>
+      <c r="D139" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
-      <c r="A140" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B140" s="7" t="s">
+      <c r="A140" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B140" s="8" t="s">
         <v>200</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D140" s="3"/>
+      <c r="D140" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
-      <c r="A141" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B141" s="7" t="s">
+      <c r="A141" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B141" s="8" t="s">
         <v>202</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D141" s="3"/>
+      <c r="D141" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
-      <c r="A142" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B142" s="7" t="s">
+      <c r="A142" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B142" s="8" t="s">
         <v>204</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D142" s="3"/>
+      <c r="D142" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
-      <c r="A143" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B143" s="7" t="s">
+      <c r="A143" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B143" s="8" t="s">
         <v>206</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D143" s="3"/>
+      <c r="D143" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
-      <c r="A144" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B144" s="7" t="s">
+      <c r="A144" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B144" s="8" t="s">
         <v>207</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D144" s="3"/>
+      <c r="D144" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
-      <c r="A145" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B145" s="8" t="s">
+      <c r="A145" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B145" s="9" t="s">
         <v>208</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D145" s="3"/>
+      <c r="D145" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
-      <c r="A146" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B146" s="8" t="s">
+      <c r="A146" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B146" s="9" t="s">
         <v>209</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D146" s="3"/>
+      <c r="D146" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
-      <c r="A147" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B147" s="8" t="s">
+      <c r="A147" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B147" s="9" t="s">
         <v>210</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D147" s="3"/>
+      <c r="D147" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
-      <c r="A148" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B148" s="8" t="s">
+      <c r="A148" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B148" s="9" t="s">
         <v>212</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D148" s="3"/>
+      <c r="D148" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
-      <c r="A149" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B149" s="8" t="s">
+      <c r="A149" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B149" s="9" t="s">
         <v>213</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D149" s="3"/>
+      <c r="D149" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
-      <c r="A150" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B150" s="8" t="s">
+      <c r="A150" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B150" s="9" t="s">
         <v>214</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D150" s="3"/>
+      <c r="D150" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
-      <c r="A151" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B151" s="8" t="s">
+      <c r="A151" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B151" s="9" t="s">
         <v>216</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D151" s="3"/>
+      <c r="D151" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
-      <c r="A152" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B152" s="8" t="s">
+      <c r="A152" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B152" s="9" t="s">
         <v>218</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D152" s="3"/>
+      <c r="D152" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
-      <c r="A153" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B153" s="8" t="s">
+      <c r="A153" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B153" s="9" t="s">
         <v>220</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D153" s="3"/>
+      <c r="D153" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
-      <c r="A154" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B154" s="8" t="s">
+      <c r="A154" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B154" s="9" t="s">
         <v>222</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D154" s="3"/>
+      <c r="D154" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
-      <c r="A155" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B155" s="8" t="s">
+      <c r="A155" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B155" s="9" t="s">
         <v>223</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D155" s="3"/>
+      <c r="D155" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
-      <c r="A156" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B156" s="8" t="s">
+      <c r="A156" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B156" s="9" t="s">
         <v>225</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D156" s="3"/>
+      <c r="D156" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
-      <c r="A157" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B157" s="8" t="s">
+      <c r="A157" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B157" s="9" t="s">
         <v>227</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D157" s="3"/>
+      <c r="D157" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
-      <c r="A158" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B158" s="8" t="s">
+      <c r="A158" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B158" s="9" t="s">
         <v>228</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D158" s="3"/>
+      <c r="D158" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
-      <c r="A159" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B159" s="8" t="s">
+      <c r="A159" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B159" s="9" t="s">
         <v>208</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D159" s="3"/>
+      <c r="D159" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
-      <c r="A160" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B160" s="8" t="s">
+      <c r="A160" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B160" s="9" t="s">
         <v>230</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D160" s="3"/>
+      <c r="D160" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
-      <c r="A161" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B161" s="8" t="s">
+      <c r="A161" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B161" s="9" t="s">
         <v>232</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D161" s="3"/>
+      <c r="D161" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
-      <c r="A162" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B162" s="8" t="s">
+      <c r="A162" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B162" s="9" t="s">
         <v>101</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D162" s="3"/>
+      <c r="D162" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
-      <c r="A163" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B163" s="8" t="s">
+      <c r="A163" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B163" s="9" t="s">
         <v>234</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="D163" s="3"/>
+      <c r="D163" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
-      <c r="A164" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B164" s="8" t="s">
+      <c r="A164" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B164" s="9" t="s">
         <v>235</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D164" s="3"/>
+      <c r="D164" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
-      <c r="A165" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B165" s="8" t="s">
+      <c r="A165" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B165" s="9" t="s">
         <v>236</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D165" s="3"/>
+      <c r="D165" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
-      <c r="A166" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B166" s="8" t="s">
+      <c r="A166" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B166" s="9" t="s">
         <v>209</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D166" s="3"/>
+      <c r="D166" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
-      <c r="A167" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B167" s="8" t="s">
+      <c r="A167" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B167" s="9" t="s">
         <v>238</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D167" s="3"/>
+      <c r="D167" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
-      <c r="A168" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B168" s="8" t="s">
+      <c r="A168" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B168" s="9" t="s">
         <v>240</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D168" s="3"/>
+      <c r="D168" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
-      <c r="A169" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B169" s="8" t="s">
+      <c r="A169" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B169" s="9" t="s">
         <v>242</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D169" s="3"/>
+      <c r="D169" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
-      <c r="A170" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B170" s="8" t="s">
+      <c r="A170" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B170" s="9" t="s">
         <v>244</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="D170" s="3"/>
+      <c r="D170" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
-      <c r="A171" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B171" s="8" t="s">
+      <c r="A171" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B171" s="9" t="s">
         <v>245</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D171" s="3"/>
+      <c r="D171" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
-      <c r="A172" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B172" s="8" t="s">
+      <c r="A172" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B172" s="9" t="s">
         <v>247</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D172" s="3"/>
+      <c r="D172" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
-      <c r="A173" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B173" s="8" t="s">
+      <c r="A173" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B173" s="9" t="s">
         <v>248</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D173" s="3"/>
+      <c r="D173" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
-      <c r="A174" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B174" s="8" t="s">
+      <c r="A174" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B174" s="9" t="s">
         <v>250</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D174" s="3"/>
+      <c r="D174" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
-      <c r="A175" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B175" s="8" t="s">
+      <c r="A175" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B175" s="9" t="s">
         <v>213</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D175" s="3"/>
+      <c r="D175" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
-      <c r="A176" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B176" s="8" t="s">
+      <c r="A176" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B176" s="9" t="s">
         <v>251</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D176" s="3"/>
+      <c r="D176" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
-      <c r="A177" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B177" s="8" t="s">
+      <c r="A177" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B177" s="9" t="s">
         <v>253</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D177" s="3"/>
+      <c r="D177" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
-      <c r="A178" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B178" s="8" t="s">
+      <c r="A178" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B178" s="9" t="s">
         <v>255</v>
       </c>
       <c r="C178" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D178" s="3"/>
+      <c r="D178" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
-      <c r="A179" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B179" s="8" t="s">
+      <c r="A179" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B179" s="9" t="s">
         <v>257</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D179" s="3"/>
+      <c r="D179" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
-      <c r="A180" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B180" s="8" t="s">
+      <c r="A180" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B180" s="9" t="s">
         <v>259</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D180" s="3"/>
+      <c r="D180" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
-      <c r="A181" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B181" s="8" t="s">
+      <c r="A181" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B181" s="9" t="s">
         <v>261</v>
       </c>
       <c r="C181" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D181" s="3"/>
+      <c r="D181" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
-      <c r="A182" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B182" s="8" t="s">
+      <c r="A182" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B182" s="9" t="s">
         <v>263</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D182" s="3"/>
+      <c r="D182" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
-      <c r="A183" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B183" s="8" t="s">
+      <c r="A183" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B183" s="9" t="s">
         <v>265</v>
       </c>
       <c r="C183" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D183" s="3"/>
+      <c r="D183" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
-      <c r="A184" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B184" s="8" t="s">
+      <c r="A184" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B184" s="9" t="s">
         <v>266</v>
       </c>
       <c r="C184" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D184" s="3"/>
+      <c r="D184" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
-      <c r="A185" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B185" s="8" t="s">
+      <c r="A185" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B185" s="9" t="s">
         <v>267</v>
       </c>
       <c r="C185" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="D185" s="3"/>
+      <c r="D185" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
-      <c r="A186" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B186" s="8" t="s">
+      <c r="A186" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B186" s="9" t="s">
         <v>269</v>
       </c>
       <c r="C186" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D186" s="3"/>
+      <c r="D186" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
-      <c r="A187" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B187" s="7" t="s">
+      <c r="A187" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B187" s="8" t="s">
         <v>270</v>
       </c>
       <c r="C187" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D187" s="3"/>
+      <c r="D187" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
-      <c r="A188" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B188" s="7" t="s">
+      <c r="A188" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188" s="8" t="s">
         <v>271</v>
       </c>
       <c r="C188" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="D188" s="3"/>
+      <c r="D188" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
-      <c r="A189" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B189" s="7" t="s">
+      <c r="A189" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B189" s="8" t="s">
         <v>272</v>
       </c>
       <c r="C189" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D189" s="3"/>
+      <c r="D189" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
-      <c r="A190" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B190" s="7" t="s">
+      <c r="A190" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190" s="8" t="s">
         <v>274</v>
       </c>
       <c r="C190" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D190" s="3"/>
+      <c r="D190" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
-      <c r="A191" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B191" s="8" t="s">
+      <c r="A191" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B191" s="9" t="s">
         <v>276</v>
       </c>
       <c r="C191" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="D191" s="3"/>
+      <c r="D191" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
-      <c r="A192" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B192" s="8" t="s">
+      <c r="A192" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192" s="9" t="s">
         <v>278</v>
       </c>
       <c r="C192" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="D192" s="3"/>
+      <c r="D192" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
-      <c r="A193" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B193" s="8" t="s">
+      <c r="A193" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B193" s="9" t="s">
         <v>280</v>
       </c>
       <c r="C193" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D193" s="3"/>
+      <c r="D193" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
-      <c r="A194" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B194" s="8" t="s">
+      <c r="A194" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B194" s="9" t="s">
         <v>281</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D194" s="3"/>
+      <c r="D194" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
-      <c r="A195" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B195" s="8" t="s">
+      <c r="A195" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B195" s="9" t="s">
         <v>282</v>
       </c>
       <c r="C195" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D195" s="3"/>
+      <c r="D195" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
-      <c r="A196" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B196" s="8" t="s">
+      <c r="A196" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B196" s="9" t="s">
         <v>283</v>
       </c>
       <c r="C196" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D196" s="3"/>
+      <c r="D196" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
-      <c r="A197" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B197" s="8" t="s">
+      <c r="A197" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B197" s="9" t="s">
         <v>284</v>
       </c>
       <c r="C197" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D197" s="3"/>
+      <c r="D197" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
-      <c r="A198" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B198" s="8" t="s">
+      <c r="A198" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198" s="9" t="s">
         <v>286</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D198" s="3"/>
+      <c r="D198" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
-      <c r="A199" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B199" s="7">
+      <c r="A199" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B199" s="8">
         <v>102730</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="D199" s="3"/>
+      <c r="D199" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
-      <c r="A200" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B200" s="7">
+      <c r="A200" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B200" s="8">
         <v>102727</v>
       </c>
       <c r="C200" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D200" s="3"/>
+      <c r="D200" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
-      <c r="A201" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B201" s="7">
+      <c r="A201" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B201" s="8">
         <v>102728</v>
       </c>
       <c r="C201" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D201" s="3"/>
+      <c r="D201" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
-      <c r="A202" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B202" s="8" t="s">
+      <c r="A202" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202" s="9" t="s">
         <v>291</v>
       </c>
       <c r="C202" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D202" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75" customFormat="1" s="9">
-      <c r="A203" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B203" s="11" t="s">
+      <c r="D202" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75" customFormat="1" s="10">
+      <c r="A203" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B203" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="C203" s="10" t="s">
+      <c r="C203" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="D203" s="10"/>
+      <c r="D203" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="18.75">
-      <c r="A204" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B204" s="13" t="s">
+      <c r="A204" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B204" s="12" t="s">
         <v>294</v>
       </c>
       <c r="C204" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="D204" s="3"/>
+      <c r="D204" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="18.75">
-      <c r="A205" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B205" s="14" t="s">
+      <c r="A205" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B205" s="8" t="s">
         <v>296</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="D205" s="3"/>
+      <c r="D205" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="18.75">
-      <c r="A206" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B206" s="14" t="s">
+      <c r="A206" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B206" s="8" t="s">
         <v>298</v>
       </c>
       <c r="C206" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D206" s="3"/>
+      <c r="D206" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18.75">
-      <c r="A207" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B207" s="8" t="s">
+      <c r="A207" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B207" s="9" t="s">
         <v>300</v>
       </c>
       <c r="C207" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D207" s="3"/>
+      <c r="D207" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>